<commit_message>
up bai tap bai 3 array_method
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym_module2/[A0321I1] TKB Advanced Programming in Java.xlsx
+++ b/TaiLieuCodegym_module2/[A0321I1] TKB Advanced Programming in Java.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-TranMinhKhoa\TaiLieuCodegym_module2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BADF8C9-D516-4799-812F-C539FB6F4F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809F1941-10EE-480C-A096-5C5AB6655031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -1387,11 +1387,12 @@
       <c r="E13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="21" t="s">
-        <v>112</v>
-      </c>
+      <c r="F13" s="21"/>
       <c r="G13" s="39" t="s">
         <v>28</v>
+      </c>
+      <c r="H13" t="s">
+        <v>112</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
@@ -1430,10 +1431,13 @@
         <v>31</v>
       </c>
       <c r="F14" s="21" t="str">
-        <f t="shared" ref="F13:F37" si="1">IF(C14="Fri","Nộp báo cáo tuần","")</f>
+        <f>IF(C14="Fri","Nộp báo cáo tuần","")</f>
         <v>Nộp báo cáo tuần</v>
       </c>
       <c r="G14" s="40"/>
+      <c r="H14" t="s">
+        <v>112</v>
+      </c>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="2"/>
@@ -1471,7 +1475,7 @@
         <v>34</v>
       </c>
       <c r="F15" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F14:F37" si="1">IF(C15="Fri","Nộp báo cáo tuần","")</f>
         <v/>
       </c>
       <c r="G15" s="40"/>

</xml_diff>

<commit_message>
up thuc hanh bai11 stack and queue using linkedlist
</commit_message>
<xml_diff>
--- a/TaiLieuCodegym_module2/[A0321I1] TKB Advanced Programming in Java.xlsx
+++ b/TaiLieuCodegym_module2/[A0321I1] TKB Advanced Programming in Java.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A0321I1-TranMinhKhoa\TaiLieuCodegym_module2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809F1941-10EE-480C-A096-5C5AB6655031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74D9B30-3742-4CBE-BA95-4D48FD1DE377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,14 +19,14 @@
   <calcPr calcId="191029"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjtB2y/5DAZBvfVsA5KxcIOrhbnmA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mhPTGSFdSI8pzPCVPJcsvfoJc2xWA=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="117">
   <si>
     <t>THỜI KHOÁ BIỂU</t>
   </si>
@@ -129,13 +129,22 @@
     <t>Buổi 3</t>
   </si>
   <si>
+    <t>thêm ngày do dịch covid</t>
+  </si>
+  <si>
+    <t>Buổi 4</t>
+  </si>
+  <si>
     <t>APJ.T3</t>
   </si>
   <si>
     <t>APJ.L3</t>
   </si>
   <si>
-    <t>Buổi 4</t>
+    <t>Buổi 5</t>
+  </si>
+  <si>
+    <t>Buổi 6</t>
   </si>
   <si>
     <t>APJ.T4</t>
@@ -144,7 +153,10 @@
     <t>APJ.L4</t>
   </si>
   <si>
-    <t>Buổi 5</t>
+    <t>Buổi 7</t>
+  </si>
+  <si>
+    <t>Buổi 8</t>
   </si>
   <si>
     <t>APJ.T5</t>
@@ -153,10 +165,10 @@
     <t>APJ.L5</t>
   </si>
   <si>
-    <t>Buổi 6</t>
+    <t>Buổi 9</t>
   </si>
   <si>
-    <t>Buổi 7</t>
+    <t>Buổi 10</t>
   </si>
   <si>
     <t>APJ.T6</t>
@@ -165,10 +177,10 @@
     <t>APJ.L6</t>
   </si>
   <si>
-    <t>Buổi 8</t>
+    <t>Buổi 11</t>
   </si>
   <si>
-    <t>Buổi 9</t>
+    <t>Buổi 12</t>
   </si>
   <si>
     <t>APJ.T7</t>
@@ -177,10 +189,10 @@
     <t>APJ.L7</t>
   </si>
   <si>
-    <t>Buổi 10</t>
+    <t>Buổi 13</t>
   </si>
   <si>
-    <t>Buổi 11</t>
+    <t>Buổi 14</t>
   </si>
   <si>
     <t>APJ.T8</t>
@@ -189,7 +201,7 @@
     <t>APJ.L8</t>
   </si>
   <si>
-    <t>Buổi 12</t>
+    <t>Buổi 15</t>
   </si>
   <si>
     <t>APJ.T10</t>
@@ -198,10 +210,10 @@
     <t>APJ.L10</t>
   </si>
   <si>
-    <t>Buổi 13</t>
+    <t>Buổi 16</t>
   </si>
   <si>
-    <t>Buổi 14</t>
+    <t>Buổi 17</t>
   </si>
   <si>
     <t>APJ.T11</t>
@@ -210,10 +222,10 @@
     <t>APJ.L11</t>
   </si>
   <si>
-    <t>Buổi 15</t>
+    <t>Buổi 18</t>
   </si>
   <si>
-    <t>Buổi 16</t>
+    <t>Buổi 19</t>
   </si>
   <si>
     <t>APJ.T12</t>
@@ -222,10 +234,10 @@
     <t>APJ.L12</t>
   </si>
   <si>
-    <t>Buổi 17</t>
+    <t>Buổi 20</t>
   </si>
   <si>
-    <t>Buổi 18</t>
+    <t>Buổi 21</t>
   </si>
   <si>
     <t>APJ.T13</t>
@@ -234,7 +246,7 @@
     <t>APJ.L13</t>
   </si>
   <si>
-    <t>Buổi 19</t>
+    <t>Buổi 22</t>
   </si>
   <si>
     <t>APJ.T14</t>
@@ -243,7 +255,7 @@
     <t>APJ.L14</t>
   </si>
   <si>
-    <t>Buổi 20</t>
+    <t>Buổi 23</t>
   </si>
   <si>
     <t>APJ.T15</t>
@@ -252,10 +264,10 @@
     <t>APJ.L15</t>
   </si>
   <si>
-    <t>Buổi 21</t>
+    <t>Buổi 24</t>
   </si>
   <si>
-    <t>Buổi 22</t>
+    <t>Buổi 25</t>
   </si>
   <si>
     <t>APJ.T16</t>
@@ -264,7 +276,7 @@
     <t>APJ.L16</t>
   </si>
   <si>
-    <t>Buổi 23</t>
+    <t>Buổi 26</t>
   </si>
   <si>
     <t>APJ.T19</t>
@@ -273,7 +285,7 @@
     <t>APJ.L19</t>
   </si>
   <si>
-    <t>Buổi 24</t>
+    <t>Buổi 27</t>
   </si>
   <si>
     <t>APJ.T20</t>
@@ -282,19 +294,19 @@
     <t>APJ.L20</t>
   </si>
   <si>
-    <t>Buổi 25</t>
+    <t>Buổi 28</t>
   </si>
   <si>
     <t>CaseStudyBS</t>
   </si>
   <si>
-    <t>Buổi 26</t>
+    <t>Buổi 29</t>
   </si>
   <si>
     <t>Retros CAH</t>
   </si>
   <si>
-    <t>Buổi 27</t>
+    <t>Buổi 30</t>
   </si>
   <si>
     <t>BP. Exam</t>
@@ -303,7 +315,7 @@
     <t>Phiếu GPA, Tự đánh giá năng lực cho Học viên, Giảng viên</t>
   </si>
   <si>
-    <t>Buổi 28</t>
+    <t>Buổi 31</t>
   </si>
   <si>
     <t>Tổng kết</t>
@@ -629,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -679,6 +691,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
@@ -701,6 +716,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -964,10 +980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -976,7 +992,7 @@
     <col min="2" max="3" width="11.453125" customWidth="1"/>
     <col min="4" max="4" width="13.81640625" customWidth="1"/>
     <col min="5" max="5" width="15.54296875" customWidth="1"/>
-    <col min="6" max="6" width="42.08984375" customWidth="1"/>
+    <col min="6" max="6" width="42.1796875" customWidth="1"/>
     <col min="7" max="7" width="24.81640625" customWidth="1"/>
     <col min="8" max="9" width="11.453125" customWidth="1"/>
     <col min="10" max="26" width="13.453125" customWidth="1"/>
@@ -1166,10 +1182,10 @@
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="2"/>
       <c r="E7" s="8" t="s">
         <v>7</v>
@@ -1202,10 +1218,10 @@
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="2"/>
       <c r="E8" s="8" t="s">
         <v>11</v>
@@ -1378,7 +1394,7 @@
         <v>44363</v>
       </c>
       <c r="C13" s="19" t="str">
-        <f t="shared" ref="C13:C40" si="0">TEXT(B13,"ddd")</f>
+        <f t="shared" ref="C13:C43" si="0">TEXT(B13,"ddd")</f>
         <v>Wed</v>
       </c>
       <c r="D13" s="20" t="s">
@@ -1387,12 +1403,15 @@
       <c r="E13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="21" t="str">
+        <f t="shared" ref="F13:F14" si="1">IF(C13="Fri","Nộp báo cáo tuần","")</f>
+        <v/>
+      </c>
+      <c r="G13" s="41" t="s">
         <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
@@ -1431,12 +1450,12 @@
         <v>31</v>
       </c>
       <c r="F14" s="21" t="str">
-        <f>IF(C14="Fri","Nộp báo cáo tuần","")</f>
+        <f t="shared" si="1"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G14" s="40"/>
+      <c r="G14" s="42"/>
       <c r="H14" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
@@ -1468,17 +1487,19 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="21" t="str">
-        <f t="shared" ref="F14:F37" si="1">IF(C15="Fri","Nộp báo cáo tuần","")</f>
-        <v/>
-      </c>
-      <c r="G15" s="40"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
       <c r="L15" s="2"/>
@@ -1499,7 +1520,7 @@
     </row>
     <row r="16" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="22">
         <f>WORKDAY(B15,IF(WEEKDAY(B15) = 2, 2,IF(WEEKDAY(B15)=4,2,IF(WEEKDAY(B15)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1510,16 +1531,15 @@
         <v>Wed</v>
       </c>
       <c r="D16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G16" s="40"/>
+      <c r="G16" s="42"/>
+      <c r="H16" t="s">
+        <v>116</v>
+      </c>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
       <c r="L16" s="2"/>
@@ -1540,7 +1560,7 @@
     </row>
     <row r="17" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="22">
         <f>WORKDAY(B16,IF(WEEKDAY(B16) = 2, 2,IF(WEEKDAY(B16)=4,2,IF(WEEKDAY(B16)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1550,17 +1570,19 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D17" s="20" t="s">
-        <v>39</v>
+      <c r="D17" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v>Nộp báo cáo tuần</v>
-      </c>
-      <c r="G17" s="40"/>
+        <v>36</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="42"/>
+      <c r="H17" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
       <c r="L17" s="2"/>
@@ -1581,7 +1603,7 @@
     </row>
     <row r="18" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="22">
         <f>WORKDAY(B17,IF(WEEKDAY(B17) = 2, 2,IF(WEEKDAY(B17)=4,2,IF(WEEKDAY(B17)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1591,17 +1613,16 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>40</v>
+      <c r="D18" s="20" t="s">
+        <v>39</v>
       </c>
       <c r="E18" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G18" s="40"/>
+      <c r="G18" s="42"/>
+      <c r="H18" t="s">
+        <v>116</v>
+      </c>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
       <c r="L18" s="2"/>
@@ -1622,7 +1643,7 @@
     </row>
     <row r="19" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="22">
         <f>WORKDAY(B18,IF(WEEKDAY(B18) = 2, 2,IF(WEEKDAY(B18)=4,2,IF(WEEKDAY(B18)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1632,17 +1653,19 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>43</v>
+      <c r="D19" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="21" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="G19" s="40"/>
+        <v>40</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="42"/>
+      <c r="H19" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
       <c r="L19" s="2"/>
@@ -1663,7 +1686,7 @@
     </row>
     <row r="20" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B20" s="22">
         <f>WORKDAY(B19,IF(WEEKDAY(B19) = 2, 2,IF(WEEKDAY(B19)=4,2,IF(WEEKDAY(B19)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1673,17 +1696,20 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>44</v>
+      <c r="D20" s="20" t="s">
+        <v>43</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>44</v>
       </c>
       <c r="F20" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F20:F40" si="2">IF(C20="Fri","Nộp báo cáo tuần","")</f>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G20" s="40"/>
+      <c r="G20" s="42"/>
+      <c r="H20" t="s">
+        <v>116</v>
+      </c>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
@@ -1704,7 +1730,7 @@
     </row>
     <row r="21" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="22">
         <f>WORKDAY(B20,IF(WEEKDAY(B20) = 2, 2,IF(WEEKDAY(B20)=4,2,IF(WEEKDAY(B20)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1714,17 +1740,20 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>47</v>
+      <c r="D21" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F21" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G21" s="40"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
       <c r="L21" s="2"/>
@@ -1745,7 +1774,7 @@
     </row>
     <row r="22" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B22" s="22">
         <f>WORKDAY(B21,IF(WEEKDAY(B21) = 2, 2,IF(WEEKDAY(B21)=4,2,IF(WEEKDAY(B21)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1755,19 +1784,22 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>48</v>
+      <c r="D22" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G22" s="40"/>
+      <c r="G22" s="42"/>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="K22" s="1"/>
       <c r="L22" s="2"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1786,7 +1818,7 @@
     </row>
     <row r="23" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B23" s="22">
         <f>WORKDAY(B22,IF(WEEKDAY(B22) = 2, 2,IF(WEEKDAY(B22)=4,2,IF(WEEKDAY(B22)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1796,19 +1828,22 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>51</v>
+      <c r="D23" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F23" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G23" s="40"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J23" s="2"/>
-      <c r="K23" s="23"/>
+      <c r="K23" s="1"/>
       <c r="L23" s="2"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
@@ -1827,7 +1862,7 @@
     </row>
     <row r="24" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" s="22">
         <f>WORKDAY(B23,IF(WEEKDAY(B23) = 2, 2,IF(WEEKDAY(B23)=4,2,IF(WEEKDAY(B23)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1838,16 +1873,19 @@
         <v>Mon</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F24" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G24" s="40"/>
+      <c r="G24" s="42"/>
+      <c r="H24" t="s">
+        <v>116</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
       <c r="L24" s="2"/>
@@ -1868,7 +1906,7 @@
     </row>
     <row r="25" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B25" s="22">
         <f>WORKDAY(B24,IF(WEEKDAY(B24) = 2, 2,IF(WEEKDAY(B24)=4,2,IF(WEEKDAY(B24)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1879,18 +1917,21 @@
         <v>Wed</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F25" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G25" s="40"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J25" s="2"/>
-      <c r="K25" s="1"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
@@ -1909,7 +1950,7 @@
     </row>
     <row r="26" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B26" s="22">
         <f>WORKDAY(B25,IF(WEEKDAY(B25) = 2, 2,IF(WEEKDAY(B25)=4,2,IF(WEEKDAY(B25)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1920,18 +1961,21 @@
         <v>Fri</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F26" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G26" s="40"/>
+      <c r="G26" s="42"/>
+      <c r="H26" t="s">
+        <v>116</v>
+      </c>
       <c r="J26" s="2"/>
-      <c r="K26" s="1"/>
+      <c r="K26" s="24"/>
       <c r="L26" s="2"/>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
@@ -1950,7 +1994,7 @@
     </row>
     <row r="27" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B27" s="22">
         <f>WORKDAY(B26,IF(WEEKDAY(B26) = 2, 2,IF(WEEKDAY(B26)=4,2,IF(WEEKDAY(B26)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -1960,17 +2004,20 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>59</v>
+      <c r="D27" s="20" t="s">
+        <v>58</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>59</v>
       </c>
       <c r="F27" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G27" s="40"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
       <c r="L27" s="2"/>
@@ -1991,7 +2038,7 @@
     </row>
     <row r="28" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B28" s="22">
         <f>WORKDAY(B27,IF(WEEKDAY(B27) = 2, 2,IF(WEEKDAY(B27)=4,2,IF(WEEKDAY(B27)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2001,17 +2048,20 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>62</v>
+      <c r="D28" s="17" t="s">
+        <v>59</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F28" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G28" s="40"/>
+      <c r="G28" s="42"/>
+      <c r="H28" t="s">
+        <v>116</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="1"/>
       <c r="L28" s="2"/>
@@ -2032,7 +2082,7 @@
     </row>
     <row r="29" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" s="22">
         <f>WORKDAY(B28,IF(WEEKDAY(B28) = 2, 2,IF(WEEKDAY(B28)=4,2,IF(WEEKDAY(B28)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2042,17 +2092,17 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>63</v>
+      <c r="D29" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>63</v>
       </c>
       <c r="F29" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G29" s="40"/>
+      <c r="G29" s="42"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1"/>
       <c r="L29" s="2"/>
@@ -2073,7 +2123,7 @@
     </row>
     <row r="30" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" s="22">
         <f>WORKDAY(B29,IF(WEEKDAY(B29) = 2, 2,IF(WEEKDAY(B29)=4,2,IF(WEEKDAY(B29)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2083,17 +2133,17 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>66</v>
+      <c r="D30" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F30" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G30" s="40"/>
+      <c r="G30" s="42"/>
       <c r="J30" s="2"/>
       <c r="K30" s="1"/>
       <c r="L30" s="2"/>
@@ -2114,7 +2164,7 @@
     </row>
     <row r="31" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B31" s="22">
         <f>WORKDAY(B30,IF(WEEKDAY(B30) = 2, 2,IF(WEEKDAY(B30)=4,2,IF(WEEKDAY(B30)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2125,16 +2175,16 @@
         <v>Wed</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F31" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G31" s="40"/>
+      <c r="G31" s="42"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1"/>
       <c r="L31" s="2"/>
@@ -2155,7 +2205,7 @@
     </row>
     <row r="32" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B32" s="22">
         <f>WORKDAY(B31,IF(WEEKDAY(B31) = 2, 2,IF(WEEKDAY(B31)=4,2,IF(WEEKDAY(B31)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2165,17 +2215,17 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>72</v>
+      <c r="D32" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F32" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G32" s="40"/>
+      <c r="G32" s="42"/>
       <c r="J32" s="2"/>
       <c r="K32" s="1"/>
       <c r="L32" s="2"/>
@@ -2196,7 +2246,7 @@
     </row>
     <row r="33" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B33" s="22">
         <f>WORKDAY(B32,IF(WEEKDAY(B32) = 2, 2,IF(WEEKDAY(B32)=4,2,IF(WEEKDAY(B32)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2206,17 +2256,17 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D33" s="17" t="s">
-        <v>73</v>
+      <c r="D33" s="20" t="s">
+        <v>70</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F33" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G33" s="40"/>
+      <c r="G33" s="42"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1"/>
       <c r="L33" s="2"/>
@@ -2237,7 +2287,7 @@
     </row>
     <row r="34" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B34" s="22">
         <f>WORKDAY(B33,IF(WEEKDAY(B33) = 2, 2,IF(WEEKDAY(B33)=4,2,IF(WEEKDAY(B33)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2248,16 +2298,16 @@
         <v>Wed</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F34" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G34" s="40"/>
+      <c r="G34" s="42"/>
       <c r="J34" s="2"/>
       <c r="K34" s="1"/>
       <c r="L34" s="2"/>
@@ -2278,7 +2328,7 @@
     </row>
     <row r="35" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B35" s="22">
         <f>WORKDAY(B34,IF(WEEKDAY(B34) = 2, 2,IF(WEEKDAY(B34)=4,2,IF(WEEKDAY(B34)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2289,16 +2339,16 @@
         <v>Fri</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F35" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Nộp báo cáo tuần</v>
       </c>
-      <c r="G35" s="40"/>
+      <c r="G35" s="42"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1"/>
       <c r="L35" s="2"/>
@@ -2319,7 +2369,7 @@
     </row>
     <row r="36" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B36" s="22">
         <f>WORKDAY(B35,IF(WEEKDAY(B35) = 2, 2,IF(WEEKDAY(B35)=4,2,IF(WEEKDAY(B35)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2329,17 +2379,17 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D36" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>83</v>
+      <c r="D36" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>77</v>
       </c>
       <c r="F36" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G36" s="40"/>
+      <c r="G36" s="42"/>
       <c r="J36" s="2"/>
       <c r="K36" s="1"/>
       <c r="L36" s="2"/>
@@ -2358,9 +2408,9 @@
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B37" s="22">
         <f>WORKDAY(B36,IF(WEEKDAY(B36) = 2, 2,IF(WEEKDAY(B36)=4,2,IF(WEEKDAY(B36)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2370,19 +2420,17 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D37" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>85</v>
+      <c r="D37" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>81</v>
       </c>
       <c r="F37" s="21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="G37" s="40"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
+      <c r="G37" s="42"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1"/>
       <c r="L37" s="2"/>
@@ -2401,9 +2449,9 @@
       <c r="Y37" s="1"/>
       <c r="Z37" s="1"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B38" s="22">
         <f>WORKDAY(B37,IF(WEEKDAY(B37) = 2, 2,IF(WEEKDAY(B37)=4,2,IF(WEEKDAY(B37)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2413,18 +2461,17 @@
         <f t="shared" si="0"/>
         <v>Fri</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="E38" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="F38" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G38" s="40"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="12"/>
+      <c r="D38" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v>Nộp báo cáo tuần</v>
+      </c>
+      <c r="G38" s="42"/>
       <c r="J38" s="2"/>
       <c r="K38" s="1"/>
       <c r="L38" s="2"/>
@@ -2443,9 +2490,9 @@
       <c r="Y38" s="1"/>
       <c r="Z38" s="1"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B39" s="22">
         <f>WORKDAY(B38,IF(WEEKDAY(B38) = 2, 2,IF(WEEKDAY(B38)=4,2,IF(WEEKDAY(B38)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2455,18 +2502,17 @@
         <f t="shared" si="0"/>
         <v>Mon</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>89</v>
+      <c r="D39" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="G39" s="40"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="F39" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G39" s="42"/>
       <c r="J39" s="2"/>
       <c r="K39" s="1"/>
       <c r="L39" s="2"/>
@@ -2485,9 +2531,9 @@
       <c r="Y39" s="1"/>
       <c r="Z39" s="1"/>
     </row>
-    <row r="40" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B40" s="22">
         <f>WORKDAY(B39,IF(WEEKDAY(B39) = 2, 2,IF(WEEKDAY(B39)=4,2,IF(WEEKDAY(B39)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
@@ -2497,17 +2543,22 @@
         <f t="shared" si="0"/>
         <v>Wed</v>
       </c>
-      <c r="D40" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="41"/>
+      <c r="D40" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E40" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="21" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="G40" s="42"/>
       <c r="H40" s="12"/>
       <c r="I40" s="12"/>
-      <c r="J40" s="1"/>
+      <c r="J40" s="2"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
+      <c r="L40" s="2"/>
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -2523,19 +2574,33 @@
       <c r="Y40" s="1"/>
       <c r="Z40" s="1"/>
     </row>
-    <row r="41" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="12"/>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B41" s="22">
+        <f>WORKDAY(B40,IF(WEEKDAY(B40) = 2, 2,IF(WEEKDAY(B40)=4,2,IF(WEEKDAY(B40)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
+        <v>44428</v>
+      </c>
+      <c r="C41" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Fri</v>
+      </c>
+      <c r="D41" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F41" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="42"/>
       <c r="H41" s="12"/>
       <c r="I41" s="12"/>
-      <c r="J41" s="1"/>
+      <c r="J41" s="2"/>
       <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
+      <c r="L41" s="2"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
@@ -2551,23 +2616,33 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31" t="s">
+    <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="22">
+        <f>WORKDAY(B41,IF(WEEKDAY(B41) = 2, 2,IF(WEEKDAY(B41)=4,2,IF(WEEKDAY(B41)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
+        <v>44431</v>
+      </c>
+      <c r="C42" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Mon</v>
+      </c>
+      <c r="D42" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="E42" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="12"/>
+      <c r="G42" s="42"/>
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
-      <c r="J42" s="1"/>
+      <c r="J42" s="2"/>
       <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="L42" s="2"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
@@ -2584,17 +2659,23 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
+      <c r="A43" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="22">
+        <f>WORKDAY(B42,IF(WEEKDAY(B42) = 2, 2,IF(WEEKDAY(B42)=4,2,IF(WEEKDAY(B42)=6,1,2))),'Holidays 2020,2021'!$B$2:$B$18)</f>
+        <v>44433</v>
+      </c>
+      <c r="C43" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v>Wed</v>
+      </c>
+      <c r="D43" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="12"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="43"/>
       <c r="H43" s="12"/>
       <c r="I43" s="12"/>
       <c r="J43" s="1"/>
@@ -2617,12 +2698,8 @@
     </row>
     <row r="44" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
-      <c r="B44" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>98</v>
-      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -2647,13 +2724,13 @@
       <c r="Y44" s="1"/>
       <c r="Z44" s="1"/>
     </row>
-    <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1" t="s">
-        <v>99</v>
+    <row r="45" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="31"/>
+      <c r="B45" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -2679,13 +2756,13 @@
       <c r="Y45" s="1"/>
       <c r="Z45" s="1"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -2711,10 +2788,14 @@
       <c r="Y46" s="1"/>
       <c r="Z46" s="1"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="B47" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>102</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2741,8 +2822,12 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="B48" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -2769,8 +2854,12 @@
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -3810,9 +3899,9 @@
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-      <c r="I86" s="1"/>
+      <c r="G86" s="12"/>
+      <c r="H86" s="12"/>
+      <c r="I86" s="12"/>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
@@ -3838,9 +3927,9 @@
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
+      <c r="G87" s="12"/>
+      <c r="H87" s="12"/>
+      <c r="I87" s="12"/>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
@@ -3866,9 +3955,9 @@
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-      <c r="I88" s="1"/>
+      <c r="G88" s="12"/>
+      <c r="H88" s="12"/>
+      <c r="I88" s="12"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
@@ -8088,88 +8177,88 @@
       <c r="Z238" s="1"/>
     </row>
     <row r="239" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A239" s="2"/>
-      <c r="B239" s="2"/>
-      <c r="C239" s="2"/>
-      <c r="D239" s="2"/>
-      <c r="E239" s="2"/>
-      <c r="F239" s="2"/>
-      <c r="G239" s="2"/>
-      <c r="H239" s="2"/>
-      <c r="I239" s="2"/>
-      <c r="J239" s="2"/>
-      <c r="K239" s="2"/>
-      <c r="L239" s="2"/>
-      <c r="M239" s="2"/>
-      <c r="N239" s="2"/>
-      <c r="O239" s="2"/>
-      <c r="P239" s="2"/>
-      <c r="Q239" s="2"/>
-      <c r="R239" s="2"/>
-      <c r="S239" s="2"/>
-      <c r="T239" s="2"/>
-      <c r="U239" s="2"/>
-      <c r="V239" s="2"/>
-      <c r="W239" s="2"/>
-      <c r="X239" s="2"/>
-      <c r="Y239" s="2"/>
-      <c r="Z239" s="2"/>
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
+      <c r="C239" s="1"/>
+      <c r="D239" s="1"/>
+      <c r="E239" s="1"/>
+      <c r="F239" s="1"/>
+      <c r="G239" s="1"/>
+      <c r="H239" s="1"/>
+      <c r="I239" s="1"/>
+      <c r="J239" s="1"/>
+      <c r="K239" s="1"/>
+      <c r="L239" s="1"/>
+      <c r="M239" s="1"/>
+      <c r="N239" s="1"/>
+      <c r="O239" s="1"/>
+      <c r="P239" s="1"/>
+      <c r="Q239" s="1"/>
+      <c r="R239" s="1"/>
+      <c r="S239" s="1"/>
+      <c r="T239" s="1"/>
+      <c r="U239" s="1"/>
+      <c r="V239" s="1"/>
+      <c r="W239" s="1"/>
+      <c r="X239" s="1"/>
+      <c r="Y239" s="1"/>
+      <c r="Z239" s="1"/>
     </row>
     <row r="240" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
-      <c r="D240" s="2"/>
-      <c r="E240" s="2"/>
-      <c r="F240" s="2"/>
-      <c r="G240" s="2"/>
-      <c r="H240" s="2"/>
-      <c r="I240" s="2"/>
-      <c r="J240" s="2"/>
-      <c r="K240" s="2"/>
-      <c r="L240" s="2"/>
-      <c r="M240" s="2"/>
-      <c r="N240" s="2"/>
-      <c r="O240" s="2"/>
-      <c r="P240" s="2"/>
-      <c r="Q240" s="2"/>
-      <c r="R240" s="2"/>
-      <c r="S240" s="2"/>
-      <c r="T240" s="2"/>
-      <c r="U240" s="2"/>
-      <c r="V240" s="2"/>
-      <c r="W240" s="2"/>
-      <c r="X240" s="2"/>
-      <c r="Y240" s="2"/>
-      <c r="Z240" s="2"/>
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
+      <c r="C240" s="1"/>
+      <c r="D240" s="1"/>
+      <c r="E240" s="1"/>
+      <c r="F240" s="1"/>
+      <c r="G240" s="1"/>
+      <c r="H240" s="1"/>
+      <c r="I240" s="1"/>
+      <c r="J240" s="1"/>
+      <c r="K240" s="1"/>
+      <c r="L240" s="1"/>
+      <c r="M240" s="1"/>
+      <c r="N240" s="1"/>
+      <c r="O240" s="1"/>
+      <c r="P240" s="1"/>
+      <c r="Q240" s="1"/>
+      <c r="R240" s="1"/>
+      <c r="S240" s="1"/>
+      <c r="T240" s="1"/>
+      <c r="U240" s="1"/>
+      <c r="V240" s="1"/>
+      <c r="W240" s="1"/>
+      <c r="X240" s="1"/>
+      <c r="Y240" s="1"/>
+      <c r="Z240" s="1"/>
     </row>
     <row r="241" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
-      <c r="D241" s="2"/>
-      <c r="E241" s="2"/>
-      <c r="F241" s="2"/>
-      <c r="G241" s="2"/>
-      <c r="H241" s="2"/>
-      <c r="I241" s="2"/>
-      <c r="J241" s="2"/>
-      <c r="K241" s="2"/>
-      <c r="L241" s="2"/>
-      <c r="M241" s="2"/>
-      <c r="N241" s="2"/>
-      <c r="O241" s="2"/>
-      <c r="P241" s="2"/>
-      <c r="Q241" s="2"/>
-      <c r="R241" s="2"/>
-      <c r="S241" s="2"/>
-      <c r="T241" s="2"/>
-      <c r="U241" s="2"/>
-      <c r="V241" s="2"/>
-      <c r="W241" s="2"/>
-      <c r="X241" s="2"/>
-      <c r="Y241" s="2"/>
-      <c r="Z241" s="2"/>
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
+      <c r="C241" s="1"/>
+      <c r="D241" s="1"/>
+      <c r="E241" s="1"/>
+      <c r="F241" s="1"/>
+      <c r="G241" s="1"/>
+      <c r="H241" s="1"/>
+      <c r="I241" s="1"/>
+      <c r="J241" s="1"/>
+      <c r="K241" s="1"/>
+      <c r="L241" s="1"/>
+      <c r="M241" s="1"/>
+      <c r="N241" s="1"/>
+      <c r="O241" s="1"/>
+      <c r="P241" s="1"/>
+      <c r="Q241" s="1"/>
+      <c r="R241" s="1"/>
+      <c r="S241" s="1"/>
+      <c r="T241" s="1"/>
+      <c r="U241" s="1"/>
+      <c r="V241" s="1"/>
+      <c r="W241" s="1"/>
+      <c r="X241" s="1"/>
+      <c r="Y241" s="1"/>
+      <c r="Z241" s="1"/>
     </row>
     <row r="242" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A242" s="2"/>
@@ -8311,9 +8400,90 @@
       <c r="Y246" s="2"/>
       <c r="Z246" s="2"/>
     </row>
-    <row r="247" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="2"/>
+      <c r="B247" s="2"/>
+      <c r="C247" s="2"/>
+      <c r="D247" s="2"/>
+      <c r="E247" s="2"/>
+      <c r="F247" s="2"/>
+      <c r="G247" s="2"/>
+      <c r="H247" s="2"/>
+      <c r="I247" s="2"/>
+      <c r="J247" s="2"/>
+      <c r="K247" s="2"/>
+      <c r="L247" s="2"/>
+      <c r="M247" s="2"/>
+      <c r="N247" s="2"/>
+      <c r="O247" s="2"/>
+      <c r="P247" s="2"/>
+      <c r="Q247" s="2"/>
+      <c r="R247" s="2"/>
+      <c r="S247" s="2"/>
+      <c r="T247" s="2"/>
+      <c r="U247" s="2"/>
+      <c r="V247" s="2"/>
+      <c r="W247" s="2"/>
+      <c r="X247" s="2"/>
+      <c r="Y247" s="2"/>
+      <c r="Z247" s="2"/>
+    </row>
+    <row r="248" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A248" s="2"/>
+      <c r="B248" s="2"/>
+      <c r="C248" s="2"/>
+      <c r="D248" s="2"/>
+      <c r="E248" s="2"/>
+      <c r="F248" s="2"/>
+      <c r="G248" s="2"/>
+      <c r="H248" s="2"/>
+      <c r="I248" s="2"/>
+      <c r="J248" s="2"/>
+      <c r="K248" s="2"/>
+      <c r="L248" s="2"/>
+      <c r="M248" s="2"/>
+      <c r="N248" s="2"/>
+      <c r="O248" s="2"/>
+      <c r="P248" s="2"/>
+      <c r="Q248" s="2"/>
+      <c r="R248" s="2"/>
+      <c r="S248" s="2"/>
+      <c r="T248" s="2"/>
+      <c r="U248" s="2"/>
+      <c r="V248" s="2"/>
+      <c r="W248" s="2"/>
+      <c r="X248" s="2"/>
+      <c r="Y248" s="2"/>
+      <c r="Z248" s="2"/>
+    </row>
+    <row r="249" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A249" s="2"/>
+      <c r="B249" s="2"/>
+      <c r="C249" s="2"/>
+      <c r="D249" s="2"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+      <c r="G249" s="2"/>
+      <c r="H249" s="2"/>
+      <c r="I249" s="2"/>
+      <c r="J249" s="2"/>
+      <c r="K249" s="2"/>
+      <c r="L249" s="2"/>
+      <c r="M249" s="2"/>
+      <c r="N249" s="2"/>
+      <c r="O249" s="2"/>
+      <c r="P249" s="2"/>
+      <c r="Q249" s="2"/>
+      <c r="R249" s="2"/>
+      <c r="S249" s="2"/>
+      <c r="T249" s="2"/>
+      <c r="U249" s="2"/>
+      <c r="V249" s="2"/>
+      <c r="W249" s="2"/>
+      <c r="X249" s="2"/>
+      <c r="Y249" s="2"/>
+      <c r="Z249" s="2"/>
+    </row>
     <row r="250" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="251" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="252" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9065,11 +9235,14 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="G13:G40"/>
+    <mergeCell ref="G13:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -9094,14 +9267,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>104</v>
+      <c r="A1" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>108</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -9125,14 +9298,14 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34">
+      <c r="A2" s="35">
         <v>1</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="36">
         <v>44197</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>105</v>
+      <c r="C2" s="37" t="s">
+        <v>109</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -9156,14 +9329,14 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34">
+      <c r="A3" s="35">
         <v>2</v>
       </c>
-      <c r="B3" s="35">
+      <c r="B3" s="36">
         <v>44235</v>
       </c>
-      <c r="C3" s="36" t="s">
-        <v>106</v>
+      <c r="C3" s="37" t="s">
+        <v>110</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -9187,14 +9360,14 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="34">
+      <c r="A4" s="35">
         <v>3</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="36">
         <v>44236</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>107</v>
+      <c r="C4" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -9218,14 +9391,14 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34">
+      <c r="A5" s="35">
         <v>4</v>
       </c>
-      <c r="B5" s="35">
+      <c r="B5" s="36">
         <v>43850</v>
       </c>
-      <c r="C5" s="36" t="s">
-        <v>107</v>
+      <c r="C5" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -9249,14 +9422,14 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="34">
+      <c r="A6" s="35">
         <v>5</v>
       </c>
-      <c r="B6" s="35">
+      <c r="B6" s="36">
         <v>44237</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>107</v>
+      <c r="C6" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -9280,14 +9453,14 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="34">
+      <c r="A7" s="35">
         <v>6</v>
       </c>
-      <c r="B7" s="35">
+      <c r="B7" s="36">
         <v>44238</v>
       </c>
-      <c r="C7" s="36" t="s">
-        <v>107</v>
+      <c r="C7" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -9311,14 +9484,14 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="34">
+      <c r="A8" s="35">
         <v>7</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="36">
         <v>44239</v>
       </c>
-      <c r="C8" s="36" t="s">
-        <v>107</v>
+      <c r="C8" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -9342,14 +9515,14 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="34">
+      <c r="A9" s="35">
         <v>8</v>
       </c>
-      <c r="B9" s="35">
+      <c r="B9" s="36">
         <v>44240</v>
       </c>
-      <c r="C9" s="36" t="s">
-        <v>107</v>
+      <c r="C9" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -9373,14 +9546,14 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="34">
+      <c r="A10" s="35">
         <v>9</v>
       </c>
-      <c r="B10" s="35">
+      <c r="B10" s="36">
         <v>44241</v>
       </c>
-      <c r="C10" s="36" t="s">
-        <v>107</v>
+      <c r="C10" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -9404,14 +9577,14 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="34">
+      <c r="A11" s="35">
         <v>10</v>
       </c>
-      <c r="B11" s="35">
+      <c r="B11" s="36">
         <v>44242</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>107</v>
+      <c r="C11" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -9435,14 +9608,14 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="34">
+      <c r="A12" s="35">
         <v>11</v>
       </c>
-      <c r="B12" s="35">
+      <c r="B12" s="36">
         <v>44243</v>
       </c>
-      <c r="C12" s="36" t="s">
-        <v>107</v>
+      <c r="C12" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -9466,14 +9639,14 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="34">
+      <c r="A13" s="35">
         <v>12</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="36">
         <v>44244</v>
       </c>
-      <c r="C13" s="36" t="s">
-        <v>107</v>
+      <c r="C13" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -9497,14 +9670,14 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="34">
+      <c r="A14" s="35">
         <v>13</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="36">
         <v>44245</v>
       </c>
-      <c r="C14" s="36" t="s">
-        <v>107</v>
+      <c r="C14" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -9528,14 +9701,14 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="34">
+      <c r="A15" s="35">
         <v>14</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="36">
         <v>44246</v>
       </c>
-      <c r="C15" s="36" t="s">
-        <v>107</v>
+      <c r="C15" s="37" t="s">
+        <v>111</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
@@ -9559,14 +9732,14 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="34">
+      <c r="A16" s="35">
         <v>15</v>
       </c>
-      <c r="B16" s="35">
+      <c r="B16" s="36">
         <v>44307</v>
       </c>
-      <c r="C16" s="36" t="s">
-        <v>108</v>
+      <c r="C16" s="37" t="s">
+        <v>112</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -9590,14 +9763,14 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="34">
+      <c r="A17" s="35">
         <v>16</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="36">
         <v>44316</v>
       </c>
-      <c r="C17" s="36" t="s">
-        <v>109</v>
+      <c r="C17" s="37" t="s">
+        <v>113</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -9621,14 +9794,14 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="34">
+      <c r="A18" s="35">
         <v>17</v>
       </c>
-      <c r="B18" s="35">
+      <c r="B18" s="36">
         <v>44317</v>
       </c>
-      <c r="C18" s="36" t="s">
-        <v>110</v>
+      <c r="C18" s="37" t="s">
+        <v>114</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -9652,14 +9825,14 @@
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="34">
+      <c r="A19" s="35">
         <v>18</v>
       </c>
-      <c r="B19" s="35">
+      <c r="B19" s="36">
         <v>44441</v>
       </c>
-      <c r="C19" s="36" t="s">
-        <v>111</v>
+      <c r="C19" s="37" t="s">
+        <v>115</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>